<commit_message>
I made an update of the parser for telegram bot orders using Python
</commit_message>
<xml_diff>
--- a/Parser/orders.xlsx
+++ b/Parser/orders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,221 +521,629 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://freelance.habr.com/tasks/593362</t>
+          <t>https://freelance.habr.com/tasks/592972</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Рефакторинг кода backend на Django + деплой на сервер</t>
+          <t>Восстановить вебсайт на django</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>django, python, docker</t>
+          <t>django, celery, redis, postgers, nginx, elasticsearch, centos, devops, docker, git</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://freelance.habr.com/tasks/593198</t>
+          <t>https://freelance.habr.com/tasks/592590</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Заменить Sendpulse на аналог sendsay, проект на python (django)</t>
+          <t>Доработка кода back-end django (middle)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>python, django</t>
+          <t>django, back-end, разработка, python</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://freelance.habr.com/tasks/592972</t>
+          <t>https://freelance.habr.com/tasks/592062</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Восстановить вебсайт на django</t>
+          <t>Разработать web приложение для просмотра аниме</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>django, celery, redis, postgers, nginx, elasticsearch, centos, devops, docker, git</t>
+          <t>бэкенд, фронтенд</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://freelance.habr.com/tasks/592590</t>
+          <t>https://freelance.habr.com/tasks/591756</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Доработка кода back-end django (middle)</t>
+          <t>Кэш сервер для API, исправить ошибки и расширить функционал Django</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>django, back-end, разработка, python</t>
+          <t>django, python</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://freelance.habr.com/tasks/592062</t>
+          <t>https://freelance.habr.com/tasks/591324</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Разработать web приложение для просмотра аниме</t>
+          <t>Разработка бэкенда туристического портала и PMS</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>бэкенд, фронтенд</t>
+          <t>python, django, postresql, elasticsearch</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://freelance.habr.com/tasks/591756</t>
+          <t>https://freelance.habr.com/tasks/590864</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Кэш сервер для API, исправить ошибки и расширить функционал Django</t>
+          <t>Доработка SaaS платформы (Python + Django)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>django, python</t>
+          <t>python, django, эквайринг</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://freelance.habr.com/tasks/591324</t>
+          <t>https://freelance.habr.com/tasks/590376</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Разработка бэкенда туристического портала и PMS</t>
+          <t>Поменять монетизацию в проекте</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>python, django, postresql, elasticsearch</t>
+          <t>django, python</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://freelance.habr.com/tasks/590864</t>
+          <t>https://freelance.habr.com/tasks/589502</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Доработка SaaS платформы (Python + Django)</t>
+          <t>Разработка б2б интернет-магазина на Django</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>python, django, эквайринг</t>
+          <t>python, django, fastapi, celery, drf, gunicorn, docker, postgresql, swagger</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://freelance.habr.com/tasks/590376</t>
+          <t>https://freelance.habr.com/tasks/589226</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Поменять монетизацию в проекте</t>
+          <t>Backend Developer</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>django, python</t>
+          <t>nestsjs, express, ruby, ruby on rails, python, django, react</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://freelance.habr.com/tasks/589502</t>
+          <t>https://freelance.habr.com/tasks/598363</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Разработка б2б интернет-магазина на Django</t>
+          <t>Внести изменения в код (Django), сделать деплой на AWS</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>python, django, fastapi, celery, drf, gunicorn, docker, postgresql, swagger</t>
+          <t>django</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://freelance.habr.com/tasks/589226</t>
+          <t>https://freelance.habr.com/tasks/598323</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Backend Developer</t>
+          <t>Помочь настроить собственные страницы в админке Django в pet-проекте</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>nestsjs, express, ruby, ruby on rails, python, django, react</t>
+          <t>python, django</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://freelance.habr.com/tasks/555303</t>
+          <t>https://freelance.habr.com/tasks/598145</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Доработать существующий код, пофиксить баги, написать новый</t>
+          <t>Написать бэкенд на джанго для небольшого pet-проекта</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>django ninja, django</t>
+          <t>бэкенд, rest api, django, backend</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>https://freelance.habr.com/tasks/598101</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Помочь установить Postgresql и настроить его с Django на windows</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>postgresql, django</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/597379</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Реализовать полнотекстовый поиск на Django и postgresql</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>python, django, postgresql, full text, fat</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/597325</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Устранение ошибки CORS Missing Allow Origin в проекте Django+Tornado</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>python, django, tornado, linux</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/596223</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Django + Ninja API: Сделать бэкенд для синхронизации сайта с royalty calendar</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>django, ninja api, git</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/594821</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Backend dev для Solana MPC Wallet</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>web3, sss, node.js, phyton, rust</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/593362</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Рефакторинг кода backend на Django + деплой на сервер</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>django, python, docker</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/598325</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Разработать на DRF отображение древовидных данных</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>django, drf, postgresql, restapi</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/597721</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Доработать сервис (только индивидуальные разработчики)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>python, django</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/597487</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Доработка сервиса за прошлой командой</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>python, django</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/597281</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Разработка проектов (ecommerce) на Django</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>django, python, ооп</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/596761</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Нужно проверить и доработать API в проекте django drf</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>django, django rest framework</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/595465</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Доработка и тех. поддержка проекта на Django</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>python, django</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/595367</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Разработка на Django</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>django, python</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/593198</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Заменить Sendpulse на аналог sendsay, проект на python (django)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>python, django</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/555303</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Доработать существующий код, пофиксить баги, написать новый</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>django ninja, django</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>https://freelance.habr.com/tasks/446435</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B33" t="inlineStr">
         <is>
           <t>Разработать бэкэнд для сайта выборов преподавательского состава</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>postgresql, redis, django, nginx, docker, linux, python</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/598517</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Разработать telegram бота для управления и продажи VPN</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>python, telegram, vless, vpn, bot, marzban, xray</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/596965</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Разработать телеграм-бота с внедренным ИИ</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>telegram, bot, ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/595407</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Разработка магазин TG-bot</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>python, tg, опыт, ответственность</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/595303</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Собрать телеграм-бота из нескольких вопросов для ниши стройка и связать с амо на nocode</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>amocrm, bot, salesbot, salebot</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/594887</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Разработать TG-бота для анализа и мониторинга кошельков в Ethereum</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>telegram, blockchain, ethereum, telegram bot</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/593832</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Консультация TELEGRAM API</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>js, node, telegram api, mtproto​, bot</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/593672</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Разработка TON-площадки в Telegram Mini App</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>блокчейн ton, telegram mini app, web3</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/593446</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Разработать чат-бота для веб-сайта</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>python, bot, chatgpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>https://freelance.habr.com/tasks/593388</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Telegram Bot для проверки постбеков</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>телеграм, бот, постбек</t>
         </is>
       </c>
     </row>

</xml_diff>